<commit_message>
Connected mongoDB & fixed tag loading late and not being scraped issue
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash\Desktop\Courses Web Scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751153B0-3F11-417F-BBF6-A393BFA19390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABB9A4-B5A7-45B9-BF09-B0E4F9FD610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>links</t>
   </si>
   <si>
-    <t>https://www.coursera.org/professional-certificates/google-data-analytics</t>
+    <t>https://www.coursera.org/professional-certificates/google-project-management?irclickid=XFtxnQ1ldxyPROYzPS3u9VCcUkFQG639OQKVxM0&amp;irgwc=1&amp;utm_medium=partners&amp;utm_source=impact&amp;utm_campaign=4807567&amp;utm_content=b2c</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/learn/meem-agile-project-management?irclickid=XFtxnQ1ldxyPROYzPS3u9VCcUkFQG6RVOQKVxM0&amp;irgwc=1&amp;utm_medium=partners&amp;utm_source=impact&amp;utm_campaign=4807567&amp;utm_content=b2c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,14 +53,6 @@
       <color rgb="FFCE9178"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,21 +72,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,7 +363,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -392,10 +382,12 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>

</xml_diff>